<commit_message>
looking in files and update ai text
</commit_message>
<xml_diff>
--- a/src/ai_text_corrected.xlsx
+++ b/src/ai_text_corrected.xlsx
@@ -329,26 +329,20 @@
 - Arbejdstagerrettigheder
 - Atomvåben
 - Økonomiske aktiviteter der understøtter bosættelser
-- Biodiversitet og dens påvirkninger
+- Biodiversitet
 - Kontroversielle våben
 - Flyselskaber
 - Fossile brændstoffer
 - Gambling
-- Schadelig miljøpraksis
-- Menneskerettigheder og relaterede problemer
+- Miljø
+- Menneskerettigheder
 - ILO-konventionsbrud
 - Internationale sanktioner og forretningsetik
-- Involvering i kernevåben
 - Israel/Palæstina
-- Klimaomstillinger
+- Klima
 - Krydstogtskibe
-- Arbejdspraksis og -rettigheder
-- Manglende klimaambitioner
-- Militært udstyr
-- Normovertrædelser relateret til menneskerettigheder
 - Principal Adverse Impacts (PAI)
 - SPU
-- Tjenester der understøtter bosættelser
 - Udnyttelse af naturressourcer
 - Usunde fødevarer
 - Våben og militærudstyr</t>
@@ -358,138 +352,114 @@
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Arbejdstagerrettigheder relateret til ILO-konvention 87
-- Biodiversitet og dens påvirkninger
+- ILO-konventionsbrud
+- Biodiversitet
 - Kontroversielle våben
 - Fossile brændstoffer
-- Fossil ekspansion
-- Gambling
-- Skadelige miljøpraksisser
-- Brud på ILO-standarder
+- Gambling
+- Skadelige miljøpraksisser
 - Israel/Palæstina
-- Krydstogtskibes indvirkning
-- Eksponering for kul (over 5%)
-- Arbejdsretter (Labour rights)
+- Krydstogtsskibe
 - Normer for ansvarlig investering
 - Principal Adverse Impacts (PAI)
-- Uholdbare fødevarer</t>
+- Usunde fødevarer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder, herunder brud på ILO-konventioner og FN Global Compact principper
 - Biodiversitet og skadelige miljøpraksisser
-- Kontroversielle våben og konflikter relateret til dem
-- Ejendomsopkøb og negative effekter på lokalsamfund
-- Flytransport og krydstogtskibe med miljøpåvirkning
+- Kontroversielle våben
+- Ejendomsopkøb
+- Flyselskaber
 - Fossile brændstoffer, herunder kul og fossil ekspansion
-- Spil og gambling industrien
-- Menneskerettigheder, herunder normbrud og internationale konventioner
-- Usunde fødevarer som investeringstype
-- Generelt manglende klimaambitioner og dårlig ledelsespraksis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Usunde fødevarer er en eksklusionsårsag for investeringer foretaget af Frederikssund.  
-- Der er ingen yderligere eksklusionsårsager nævnt.  </t>
-  </si>
-  <si>
-    <t>- Arbejdstagerrettigheder
-- Brud på grundlæggende arbejdstagerrettigheder
+- Gambling
+- Menneskerettigheder
+- Usunde fødevarer
+- Manglende klimaambitioner
+- Israel/Palæstina
+- Krydstogtsskibe
+- Ledelsespraksis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Usunde fødevarer  </t>
+  </si>
+  <si>
+    <t>- Arbejdstagerrettigheder
 - Overtrædelse af ILO-konventionen
 - Kontroversielle våben
 - Flyselskaber
 - Menneskerettigheder
-- ILO-brud
-- Krænkelse af menneskerettigheder
 - Manglende klimaambitioner
 - Normer og normovertrædelser
 - Principal Adverse Impacts (PAI)
 - Involvering i tobaksprodukter
 - Levering af tjenester og faciliteter, der understøtter bosættelser
-- Levering af sikkerhedstjenester og udstyr til virksomheder i bosættelser
 - Udnyttelse af naturressourcer, særligt vand og land
 - Usunde fødevarer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Brud på grundlæggende arbejdstagerrettigheder (herunder ILO-konventionen 87)
-- Brud på FN Global Compact principperne 3 og 4
 - Kontroversielle våben
 - Flyselskaber
 - Israel/Palæstina
 - Manglende klimaambitioner
-- Krænkelse af menneskerettigheder
+- Menneskerettigheder
 - Principal Adverse Impacts (PAI)
 - Engagement i tobaksprodukter
-- Levering af tjenester til settlementer
-- Levering af sikkerhedstjenester til virksomheder i settlementer
-- Udvinding af termisk kul
+- Fossile brændstoffer
 - Usunde fødevarer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Brud på grundlæggende arbejdstagerrettigheder
 - Biodiversitet
 - Kontroversielle våben
 - Ejendomsopkøb
-- Fossile brændstoffer og fossil ekspansion
-- Gambling
-- Dårlig ledelsespraksis
+- Gambling
+- Ledelsespraksis
 - Skadelige miljømæssige praksisser
-- Menneskerettighedsspørgsmål
+- Menneskerettigheder
 - Brud på internationale normer og konventioner
 - Israel/Palæstina
-- Normbrud og normovertrædelser
-- Uholdbare klimaambitioner
+- Manglende klimaambitioner
 - Usunde fødevarer
 - Krydstogtskibe
-- Kul-eksponering
-- Termisk kuludvinding
 - Flyselskaber
 - Våben</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Biodiversitet og miljøpåvirkninger
-- Brud på grundlæggende arbejdstagerrettigheder i strid med FN Global Compact
+- Biodiversitet
 - Ejendomsopkøb
 - Flyselskaber
 - Fossile brændstoffer
 - Gambling
 - Skadelige miljøpraksisser
-- Menneskerettigheder og relaterede problemstillinger
+- Menneskerettigheder.
 - ILO-brud
 - Overtrædelse af internationale normer og konventioner
-- Konflikter med UN Global Compact
 - Kontroversielle våben
 - Krydstogtskibe
 - Manglende klimaambitioner
 - Usunde fødevarer
-- Udtømning af termisk kul
 - Normbrud og dårlig overholdelse af normer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Brud på menneskerettigheder (FN Global Compact Princip 1 og 2)
-- Kontroversielle våben (herunder hvidt fosfor)
+- Menneskerettigheder
+- Kontroversielle våben
 - Dårlig regeringsførelse
-- EU-sanktioner
-- Eksklusion af lande under internationale sanktioner eller vurderet ikke-investeringsegnede
-- Emerging Markets statsobligationer der ikke lever op til ESG-kriterier
-- Fossile brændsler (oliesk Sands, thermal coal extraction)
-- Udfordringer i forbindelse med landepolitik
-- Menneskerettighedskrænkelser
-- Norms violation relateret til miljøforurening og sikkerhedsstandarder
-- Usunde fødevarer
-- Utilstrækkelig tilgang til forvaltning og regeringsførelse</t>
+- Sortlistede lande
+- Fossile brændstoffer
+- Miljøforurening
+- Usunde fødevarer</t>
   </si>
   <si>
     <t>- Alkohol
 - Arbejdstagerrettigheder
 - Atomvåben
 - Biodiversitet
-- Brud på grundlæggende arbejdstagerrettigheder
 - Kontroversielle våben (inkl. hvidt fosfor)
 - Ejendomsopkøb
-- Fossile brændstoffer (kul og transition)
+- Fossile brændstoffer
 - Gambling
 - Miljømæssige skadelige praksisser 
 - Menneskerettigheder
@@ -498,25 +468,22 @@
 - Manglende klimaambitioner
 - Miljø
 - Usunde fødevarer
-- Våben og militært udstyr</t>
-  </si>
-  <si>
-    <t>- Arbejdstagerrettigheder og brud herpå, inkl. ILO-konventionen
+- Våben og militært udstyr
+- Støtte af bosættelser</t>
+  </si>
+  <si>
+    <t>- Arbejdestagerrettigheder
 - Biodiversitetspåvirkninger
 - Kontroversielle våben
 - Flyselskaber
-- Fossile brændstoffer og deres ekspansion
+- Fossile brændstoffer
 - Gambling
 - Skadelige miljøpraksisser
 - Menneskerettigheder og krænkelse heraf
 - Manglende klimaambitioner
-- Normovertrædelser
-- Negative påvirkninger relateret til menneskerettigheder
 - Involvering i tobaksprodukter
-- Tjenester og forsyninger, der understøtter bosættelser
-- Sikkerhedstjenester til virksomheder i bosættelser
+- Støtte til bosættelser
 - Udvinding af termisk kul
-- Eksponering for kul (over 5%)
 - Usunde fødevarer</t>
   </si>
   <si>
@@ -524,122 +491,95 @@
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Brud på grundlæggende arbejdstagerrettigheder
 - Overtrædelse af ILO-konventioner
 - Kontroversielle våben
 - Flyselskaber
 - Menneskerettigheder
 - Manglende klimaambitioner
-- Krænkelse af menneskerettigheder
-- Negativ påvirkning af væsentlige faktorer (Principal Adverse Impacts - PAI)
+- Principal Adverse Impacts - PAI
 - Involvering i tobaksprodukter
-- Levering af tjenester og forsyninger til bosættelser
-- Levering af sikkerhedstjenester til virksomheder i bosættelser
+- Støtte til bosættelser
 - Usunde fødevarer</t>
   </si>
   <si>
     <t>- Alkohol
 - Arbejdstagerrettigheder
 - Biodiversitet
-- Brud på menneskerettigheder (FN Global Compact Princip 1 og 2)
 - Kontroversielle våben
 - Dårlig regeringsførelse
-- EU-sanktioner
-- Udsatte lande under internationale sanktioner
-- Dårlig ESG-performance
-- Flyselskaber
-- Fossil energi (fracking, olie sand, overgang, ekspansion)
+- Sortlistede lande
+- Flyselskaber
+- Fossile brændstoffer
 - Gambling
 - Israel-Palæstina konflikten
 - Klima- og miljøforhold
 - Krydstogtskibe
-- Uholdbar landepolitik
 - Menneskerettigheder
 - Militær udstyr
 - Miljø og sundhedsnormer
-- Olie og gas (udvinding og produktion)
-- Gambling
-- Risikovurdering af ESG-forhold
+- Gambling
 - Skat og EU's sortliste
-- Tar sands
-- Tjenester der understøtter bosættelser
-- Brug af naturressourcer (vand og land)
-- Thermal coal extraction
-- Usunde fødevarer
-- Utilfredsstillende regeringsførelse og forvaltningspraksis
-- Årsag ikke nævnt</t>
+- Støtte af bosættelser
+- Usunde fødevarer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder og relaterede brud, herunder ILO-konventionen.
-- Krænkelser af menneskerettigheder, herunder forhold relateret til FN Global Compact.
-- Involvering i produktion og handel med kontroversielle våben, såsom hvid fosfor.
-- Deltagelse i aktiviteter relateret til flyselskaber.
-- Manglende klimaambitioner og usunde fødevarer.
+- Menneskerettigheder
+- Kontroversille våben - herunder hvidt fosfor
+- Flyselskaber.
+- Manglende klimaambitioner
 - Engagement i tobaksprodukter og relaterede tjenester.
-- Inddragelse i forsyning af sikkerhedstjenester til virksomheder i besatte områder.
-- Ulemper ved brug af naturlige ressourcer til kommercielle formål.</t>
-  </si>
-  <si>
-    <t>- Arbejdstagerrettigheder
-- Brud på grundlæggende arbejdstagerrettigheder
-- Produktion af kontroversielle våben, herunder hvidt fosfor
-- Involvering i flyselskab
-- Krænkelse af menneskerettigheder
-- Manglende klimatiltag
-- Uetisk produktion af tobaksprodukter
-- Levering af sikkerhedstjenester til virksomheder i omstridte områder
-- Udvinding af termisk kul
-- Distribution af usunde fødevarer</t>
-  </si>
-  <si>
-    <t>- Arbejdstagerrettigheder
-- Arbejdstagerrettigheder ifølge ILO-konventionen 87
-- Biodiversitet
-- Indvirkning på biodiversiteten
-- Kontroversielle våben
+- Støtte til virksomheder i besatte områder
+- Usunde fødevarer</t>
+  </si>
+  <si>
+    <t>- Arbejdstagerrettigheder
+- Kontroversielle våben
+- Flyselskaber
+- Menneskerettigheder
+- Manglende klimaambitioner
+- Tobak
+- Støtte til bosættelser
 - Fossile brændstoffer
-- Udvidelse af fossile brændstoffer
-- Spillespil
+- Usunde fødevarer</t>
+  </si>
+  <si>
+    <t>- Arbejdstagerrettigheder
+- Biodiversitet
+- Kontroversielle våben
+- Fossile brændstoffer
+- Gambling
 - Skadelige miljøpraksisser
 - Brud på ILO-standarder
 - Israel/Palæstina
 - Krydstogtskibe
-- Kul-eksponering over 5%
-- Arbejdsrettigheder
 - Normer
 - Principal Adverse Impacts (PAI)
-- Udrulning af termisk kul
 - Usunde fødevarer</t>
   </si>
   <si>
-    <t>- Alkohol
+    <t xml:space="preserve">- Alkohol
 - Arbejdstagerrettigheder, herunder brud på ILO-konventionen 87
 - Atomvåben og kontroversielle våben
 - Finansielle operationer der støtter bosættelser
 - Biodiversitet
-- Brud på grundlæggende arbejdstagerrettigheder og menneskerettigheder, i strid med FN Global Compact 
-- Dårlig regeringsførelse
-- EU-sanktioner og rapportering om dem
-- Ejendomsopkøb i sanktionerede lande
-- Emerging Markets statsobligationer uden ESG-overholdelse
+- Menneskerettigheder 
+- Sortlistede lande
+- Ejendomsopkøb
 - Fossil energiproduktion og ekspansion, herunder kul og olie
 - Gambling
-- God ledelsespraksis
-- Skadelige miljøpraksisser
-- Israel/Palæstina-relaterede forhold
-- Klimarelaterede forhold og manglende ambitioner
-- Normovertrædelser relateret til menneskerettigheder og miljø
+- Ledelsespraksis
+- Skadelige miljøpraksisser
+- Israel/Palæstina
+- Manglende klimaambitioner
 - Sikkerhedsforhold
 - Skat og EU's sortliste for skattepraksis
 - Usunde fødevarer
-- Vurdering af landets forvaltning og ledelsespraksis
-- Våbenhandel 
-- Ingen relevante data.</t>
-  </si>
-  <si>
-    <t>- Arbejdstagerrettigheder
-- Brud på arbejdstagerrettigheder ifølge ILO og FN Global Compact
-- Biodiversitet og biodiversitetspåvirkninger
+- Våben </t>
+  </si>
+  <si>
+    <t>- Arbejdstagerrettigheder
+- Biodiversitet
 - Kontroversielle våben
 - Flyselskaber
 - Fossile brændstoffer og fossil ekspansion
@@ -649,53 +589,37 @@
 - ILO-brud
 - Israel/Palæstina
 - Krydstogtskibe
-- Kul (kul-eksponering over 5%)
-- Manglende klimaambitioner
-- Normovertrædelser vedrørende menneskerettigheder
+- Manglende klimaambitioner
 - Principal Adverse Impacts (PAI)
 - Involvering i tobaksprodukter
-- Levering af tjenester og forsyninger til bosættelser
-- Levering af sikkerhedstjenester til virksomheder i bosættelser
-- Brug af naturressourcer som vand og land til forretningsformål
-- Uddragning af termisk kul
+- Støtte til bosættelser
 - Usunde fødevarer</t>
   </si>
   <si>
     <t xml:space="preserve">- Arbejdstagerrettigheder
-- Brud på grundlæggende arbejdstagerrettigheder 
 - Overtrædelser af ILO-konventioner 
 - Kontroversielle våben 
 - Flyselskaber 
 - Menneskerettigheder 
-- Normviolationer relateret til menneskerettigheder 
 - Manglende klimaambitioner 
 - Usunde fødevarer 
-- Anvendelse af naturressourcer til erhvervsmæssige formål 
-- Levering af sikkerhedstjenester til virksomheder i bosættelser 
-- Ydelse af transport og forbindelser til bosættelser </t>
-  </si>
-  <si>
-    <t>- Arbejdstagerrettigheder
-- Brud på arbejdstagerrettigheder (f.eks. ILO-konventionen 87)
-- Biodiversitet og dens indvirkninger
-- Brud på menneskerettigheder (f.eks. FN Global Compact Princip 1 og 2)
-- Kontroversielle våben
-- Dårlig regeringsførelse
-- EU-sanktioner
-- Lande underlagt internationale sanktioner og vurderet som ikke-investeringsegnede
-- Emerging Markets statsobligationer uden ESG-kriterier
-- Flyselskaber
-- Fossil brændstof (olie sand, kul, fossil ekspansion)
+- Støtte af bosættelser </t>
+  </si>
+  <si>
+    <t>- Arbejdstagerrettigheder
+- Biodiversitet
+- Menneskerettigheder
+- Kontroversielle våben
+- Sortlistede lande
+- Flyselskaber
+- Fossile brændstoffer
 - Gambling
 - Skadelige miljøpraksisser
 - Israel/Palæstina
-- Landepolitik
-- Normovertrædelser relateret til miljøforurening og sundheds- og sikkerhedsstandarder
 - Principal Adverse Impacts (PAI)
 - Sikkerhedsforhold
 - Skat (herunder EU's sortliste)
-- Usunde fødevarer
-- Utilfredsstillende regeringsførelse og forvaltningspraksis</t>
+- Usunde fødevarer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
@@ -709,11 +633,9 @@
 - Skadelige miljøpraksisser
 - Israel/Palæstina
 - Krydstogtskibe
-- Kul (kul-eksponering &gt; 5%)
-- Usunde fødevarer
-- Normer
+- Usunde fødevarer
 - Principal Adverse Impacts (PAI)
-- Tjenester og forsyninger, der understøtter bosættelser, herunder transport</t>
+- Støtte til bosættelser</t>
   </si>
   <si>
     <t>Der ikke er noget relevant data.</t>
@@ -721,56 +643,43 @@
   <si>
     <t>- Brud på arbejdstagerrettigheder, herunder ILO-konventionen
 - Krænkelse af menneskerettigheder
-- Overtrædelser af FN Global Compact principper
-- Investeringer i kontroversielle våben
-- Engageret i flyselskabssektoren
+- Kontroversielle våben
+- Flyselskaber
 - Manglende klimaambitioner fra virksomheder
 - Involvering i tobaksprodukter
-- Levering af tjenester og ressourcer til bosættelser
-- Levering af sikkerhedstjenester til bosættelser
-- Udnyttelse af naturressourcer, som vand og jord, til erhvervsmæssig brug
-- Producent eller distributør af usunde fødevarer</t>
-  </si>
-  <si>
-    <t>- Arbejdstagerrettigheder
-- Brud på grundlæggende arbejdstagerrettigheder
+- Støtte til bosættelser
+- Usunde fødevarer</t>
+  </si>
+  <si>
+    <t>- Arbejdstagerrettigheder
 - Overtrædelse af ILO-konventioner
 - Kontroversielle våben
 - Flyselskaber
 - Krænkelse af menneskerettigheder
 - Manglende klimaambitioner
-- Normovertrædelser relateret til menneskerettigheder
-- Principielle negative virkninger (PAI)
 - Involvering i tobaksprodukter
-- Levering af tjenester, der understøtter bosættelser
-- Levering af sikkerhedstjenester til bosættelser
-- Anvendelse af naturressourcer til kommercielle formål
+- Støtte til bosættelser
 - Usunde fødevarer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Brud på arbejdstagerrettigheder ifølge FN Global Compact
 - Biodiversitet og dets påvirkninger
 - Kontroversielle våben
-- Overtrædelse af EU-sanktioner
-- Ejendomsopkøb i konfliktområder
-- Emerging Markets statsobligationer uden ESG-kriterier
+- Sortlistede lande
+- Ejendomsopkøb
 - Flyselskaber
 - Fossile brændstoffer
 - Gambling
-- God ledelsespraksis
-- Skadelige miljøpraksisser
-- Menneskerettigheder og deres krænkelser
+- Ledelsespraksis
+- Skadelige miljøpraksisser
+- Menneskerettigheder
 - ILO-brud
-- Overtrædelse af internationale normer og konventioner
 - Israel/Palæstina
 - Manglende klimaambitioner
 - Usunde fødevarer
-- Thermal kuludvinding
+- Fossile brændstoffer
 - Involvering i tobaksprodukter
-- Levering af sikkerhedstjenester til virksomheder i bosættelser
-- Udnyttelse af naturressourcer til erhvervsformål
-- Transportmidler til vedligeholdelse af bosættelser</t>
+- TStøtte til bosættelser</t>
   </si>
   <si>
     <t>- Eksklusionsårsager ved investeringer i Region Hovedstaden inkluderer:
@@ -781,78 +690,65 @@
   - Flyselskaber
   - Krydstogtskibe
   - Normer
-  - Negative påvirkninger (Principal Adverse Impacts, PAI)
-  - Tjenester og forsyninger til opretholdelse af bosættelser, herunder transport</t>
+  - Principal Adverse Impacts, PAI
+  - Støtte til bosættelser</t>
   </si>
   <si>
     <t>- Brud på arbejdstagerrettigheder, herunder ILO-konventioner og FN Global Compact principper
 - Krænkelse af menneskerettigheder
 - Kontroversielle våben, herunder atomvåben og klyngevåben
-- Investeringer i flyselskaber og krydstogtskibe
-- Manglende klimaambitioner
-- Involvering i tobaksprodukter og usunde fødevarer
-- Levering af tjenester og forsyninger til bosættelser, herunder transport
-- Forsyning af sikkerhedstjenester til virksomheder i bosættelser
-- Anvendelse af naturlige ressourcer til erhvervsmæssige formål, særligt vand og land</t>
-  </si>
-  <si>
-    <t>- Arbejdstagerrettigheder
-- Brud på grundlæggende arbejdstagerrettigheder
+- Flyselskaber
+- Manglende klimaambitioner
+- Tobak
+- Usunde fødevarer
+- Støtte til bosættelser</t>
+  </si>
+  <si>
+    <t>- Brud på grundlæggende arbejdstagerrettigheder
 - Biodiversitet og dens påvirkninger
-- Kontroversielle våben, herunder hvid fosfor
+- Kontroversielle våben
 - EU-sanktioner
 - Ejendomsopkøb
-- Statsobligationer fra Emerging Markets, der ikke lever op til ESG-kriterier
-- Flyselskaber
-- Fossile brændstoffer og deres ekspansion
-- Gambling
-- God ledelsespraksis
-- Skadelige miljøpraksisser
-- Menneskerettighedsspørgsmål
+- Statsobligationer, der ikke lever op til ESG-kriterier
+- Flyselskaber
+- Fossile brændstoffer
+- Gambling
+- Skadelige miljøpraksisser
+- Menneskerettigheder
 - Internationale normer og konventioner
 - Israel/Palæstina
 - Normbrud relateret til miljø
 - Manglende klimaambitioner
-- Anvendelse af naturressourcer, især vand og land, til forretningsformål
 - Krydstogtskibe
-- Kul-eksponering
 - Usunde fødevarer</t>
   </si>
   <si>
-    <t>- Arbejdstagerrettigheder
-- Biodiversitet
+    <t>- Biodiversitet
 - Brud på grundlæggende arbejdstagerrettigheder
 - Kontroversielle våben
 - Fossil brændstof og ekspansion
 - Gambling
 - Skadelige miljøpraksisser
-- Menneskerettigheder
 - ILO-brud
 - Israel/Palæstina
 - Krydstogtskibe
-- Kul (kul-eksponering &gt; 5%)
 - Manglende klimaambitioner
 - Krænkelse af menneskerettigheder
-- Tobacco Products Retail (produktinddragelse)
-- Adverse impacts på menneskerettigheder og normer
-- Levering af tjenester til settlements
-- Levering af sikkerhedstjenester til virksomheder i settlements
+- Tobak
+- Støtte til virksomheder i besatte områder
 - Brug af naturressourcer (vand og land)
-- Udsigt til varme kul
 - Usunde fødevarer</t>
   </si>
   <si>
-    <t>- Arbejdstagerrettigheder og brud herpå, bl.a. ifølge ILO og FN Global Compact
+    <t>- Brud på grundlæggende arbejdstagerrettigheder
 - Biodiversitet og skadelige miljøpraksisser
-- Kontroversielle våben, herunder hvid fosfor
-- Ejendomsoverdragelser og landepolitik
+- Kontroversielle våben
+- Landepolitik
 - Investeringer i statsobligationer fra emerging markets uden ESG-kriterier
-- Deltagelse i eller støtte til flyselskaber
-- Fossile brændstoffer og kuludvinding, herunder transition og eksponering
-- God ledelsespraksis og normovertrædelser på arbejdsmarkedet
-- Menneskerettigheder og generelle human rights issues
-- Miljømæssige krav og relaterede normer
-- Adverse impacts, herunder principal adverse impacts (PAI)
+- Flyselskaber
+- Fossile brændstoffer
+- Menneskerettigheder
+- Miljø
 - Usunde fødevarer og deres indvirkning på sundhed</t>
   </si>
   <si>
@@ -862,9 +758,8 @@
 - Kontroversielle våben
 - Fossile brændstoffer
 - Udvidelse af fossile ressourcer
-- Spilaktiviteter
-- Skadelige miljøpraksisser
-- ILO-brud
+- Gambling
+- Skadelige miljøpraksisser
 - Israel/Palæstina
 - Krydstogtskibe
 - Kul (kul-eksponering over 5%)
@@ -876,9 +771,7 @@
   <si>
     <t>- Arbejdstagerrettigheder, herunder brud på ILO-konventioner
 - Biodiversitet
-- Brud på grundlæggende arbejdstagerrettigheder, stridende imod FN Global Compact principper
-- Kontroversielle våben, herunder hvid fosfor
-- Ejendomsopkøb relateret til internationale normer
+- Ejendomsopkøb
 - Involvering i produktion af hvidt fosfor
 - Israel/Palæstina
 - Konflikter med UN Global Compact principker
@@ -887,19 +780,17 @@
 - Menneskerettighedskrænkelser
 - Skadelige miljøpraksisser
 - Manglende klimaambitioner
-- Dårlig ledelsespraksis
 - Normbrud og normovertrædelser</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
 - Biodiversitet
 - Brud på grundlæggende arbejdstagerrettigheder (FN Global Compact princip 3 og 4)
-- Kontroversielle våben (herunder hvidt fosfor)
+- Kontroversielle våben
 - Ejendomsopkøb
 - Flyselskaber
 - Fossile brændstoffer
 - Gambling
-- God ledelsespraksis
 - Skadelige miljøpraksisser
 - Menneskerettigheder
 - ILO-brud
@@ -922,7 +813,6 @@
 - ILO-brud
 - Israel/Palæstina
 - Krydstogtskibe
-- Kul (kul-eksponering &gt; 5%)
 - Menneskerettigheder
 - Normer
 - Principal Adverse Impacts (PAI)
@@ -932,25 +822,22 @@
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Brud på grundlænde arbejdstagerrettigheder
+- Brud på grundlæggende arbejdstagerrettigheder
 - Kontroversielle våben
 - Flyselskaber
 - Menneskerettigheder
 - ILO-brud
 - Manglende klimaambitioner
 - Normovertrædelser
-- Principielle negative virkninger (PAI)
 - Involvering i tobaksprodukter
-- Tjenester og forsyninger til vedligeholdelse af beboelser, herunder transport
-- Levering af sikkerhedstjenester til virksomheder i beboelser
+- Støtte til virksomheder i besatte områder
 - Anvendelse af naturressourcer, især vand og land, til forretningsformål
 - Usunde fødevarer</t>
   </si>
   <si>
-    <t>- Arbejdstagerrettigheder
-- Biodiversitet
+    <t>- Biodiversitet
 - Brud på arbejdstagerrettigheder
-- Kontroversielle våben (herunder hvidt fosfor)
+- Kontroversielle våben
 - Ejendomsopkøb
 - Fossil energi (inkl. kul-eksponering)
 - Gambling
@@ -959,15 +846,14 @@
 - Menneskerettighedsproblemer
 - ILO-brud
 - Internationale normer og konventioner
-- Konflikter relateret til Israel/Palæstina
+- Israel/Palæstina
 - Manglende klimaambitioner
 - Usunde fødevarer
 - Forsyning af tjenester og forsyninger til etablering af bosættelser</t>
   </si>
   <si>
     <t>- Alkohol
-- Arbejdstagerrettigheder
-- Arbejdstagerrettigheder (inkl. ILO-konventionen 87)
+ (inkl. ILO-konventionen 87)
 - Biodiversitet og dens påvirkninger
 - Brud på grundlæggende arbejdstagerrettigheder (strider imod FN Global Compact princip 3 og 4)
 - Kontroversielle våben
@@ -977,25 +863,19 @@
 - Flyselskaber
 - Fossile brændstoffer (fracking og transition)
 - Gambling
-- God ledelsespraksis
-- Skadelige miljøpraksisser
-- Menneskerettigheder og relaterede emner
+- Skadelige miljøpraksisser
+- Menneskerettigheder
 - ILO-brud
-- Integreret olie- og gasproduktion
+- Integreret olie og gas
 - Internationale normer og konventioner
-- Klimaforhold og omstilling
+- Klimarelaterede forhold
 - Konflikt med UN Global Compact princip nr. 10
 - Krydstogtskibe
-- Kul (kul-eksponering &gt; 5%)
-- Manglende klimaambitioner
-- Miljøet
-- Normbrud og normovertrædelser
-- Olieudvinding og -produktion
+- Miljø
+- Olie- og gasudvinding samt produktion af disse
 - Principal Adverse Impacts (PAI)
-- Tobaksprodukter (detailhandel)
-- Tjenester til understøttelse af beboelser (transport mv.)
-- Forsyning af sikkerhedstjenester til virksomheder i beboelser
-- Termisk kuludvinding
+- Tobak
+- Støtte til virksomheder i besatte områder
 - Usunde fødevarer
 - Våben</t>
   </si>
@@ -1008,14 +888,14 @@
 - Flyselskaber
 - Menneskerettigheder
 - ILO-brud
-- Krænkelse af menneskerettigheder
-- Manglende klimaambitioner
-- Normovertrædelser
+- Menneskerettigheder
+- Manglende klimaambitioner
+- Normer
 - Principal Adverse Impacts (PAI)
-- Involvering i tobaksprodukter
-- Tjenester og forsyninger knyttet til opretholdelse af bosættelser
-- Levering af sikkerhedstjenester og -udstyr til virksomheder i bosættelser
-- Udnyttelse af naturressourcer, især vand og jord
+- Tobak
+- Støtte til tjenester og forsyninger i besættelsesområder
+- Støtte til sikkerhedstjenester og udstyr i besættelsesområder
+- Udnyttelse af naturressourcer, især vand og jord, til forretningsbrug, til forretningsbrug, til forretningsbrug
 - Usunde fødevarer</t>
   </si>
   <si>
@@ -1028,7 +908,7 @@
 - Fossile brændstoffer
 - Gambling
 - Skadelige miljøpraksisser
-- Menneskerettighedsspørgsmål
+- Menneskerettigheder
 - ILO-brud
 - Internationale normer og konventioner
 - Konflikt med UN Global Compact princip nr. 10
@@ -1037,13 +917,13 @@
 - Usunde fødevarer
 - Thermal coal extraction
 - Principal Adverse Impacts (PAI)
-- Normbrud og normviolationer</t>
+- Normer og normbrud</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
 - Brud på arbejdstagerrettigheder
 - Biodiversitet
-- Kontroversielle våben (herunder hvidt fosfor)
+- Kontroversielle våben
 - Ejendomsopkøb og involvering i besættelsesområder
 - Flyselskaber
 - Fossile brændstoffer (inkl. kul-eksponering)
@@ -1074,7 +954,7 @@
 - Skadelige miljøpraksisser
 - Israel/Palæstina
 - Krydstogtskibe
-- Kulkraft (kul-eksponering &gt; 5%)
+- Kul (kul-eksponering &gt; 5%)
 - Usunde fødevarer
 - Overtrædelser af ILO-konventionen
 - Primære negative påvirkninger (PAI)
@@ -1082,33 +962,32 @@
   </si>
   <si>
     <t>- Arbejdstagerrettigheder: Overtrædelser af grundlæggende rettigheder i arbejdet.
-- Brud på ILO-konventioner, især konvention 87.
+- Brud på ILO-konventioner, bl.a. konvention 87
 - Overtrædelser der strider imod FN Global Compact principper (3 og 4).
 - Kontroversielle våben: Investeringer relateret til produktion og salg.
-- Flyselskaber: Involvering med flyselskaber, der ikke opfylder etiske standarder.
-- Krænkelse af menneskerettigheder: Uretfærdig behandling af individer.
-- Normovertrædelser: Handlinger der ikke stemmer overens med internationale normer.
-- Manglende klimaambitioner: Utilstrækkelige tiltag mod klimaforandringer.
-- Usunde fødevarer: Engagement i produktion eller salg af usunde kostprodukter.
-- Tjenester der understøtter bosættelser: Involvering i serviceleverancer til omstridte områder.
+- Flyselskaber
+- Menneskerettigheder
+- Normer
+- Manglende klimaambitioner
+- Usunde fødevarer
+- Støtte til tjenester og forsyninger i besættelsesområder
 - Leverance af sikkerhedstjenester til virksomheder i bosættelser: Investeringer der bidrager til konfliktområder.</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
 - Biodiversitet
 - Brud på grundlæggende arbejdstagerrettigheder
-- Kontroversielle våben (herunder hvid fosfor)
+- Kontroversielle våben
 - Ejendomsopkøb
-- Indflydelse fra flyselskaber
+- Flyselskaber
 - Fossil brændstof
 - Gambling
 - Skadelige miljøpraksisser
-- Menneskerettigheder og tilknyttede problemstillinger
+- Menneskerettigheder
 - ILO-brud
 - Overtrædelse af internationale normer og konventioner
 - Overholdelse af internationale sanktioner og forretningsetik
-- Involvering i atomvåben
-- Krænkelse af menneskerettigheder
+- Atomvåben
 - Manglende klimaambitioner
 - Principal Adverse Impacts (PAI)
 - Sikkerhedsforhold
@@ -1121,17 +1000,16 @@
     <t>- Arbejdstagerrettigheder
 - Brud på grundlæggende arbejdstagerrettigheder
 - Biodiversitet
-- Kontroversielle våben (herunder hvid fosfor)
+- Kontroversielle våben
 - EU-sanktioner
 - Ejendomsopkøb
 - Statsobligationer fra emerging markets uden ESG-kriterier
 - Flyselskaber
-- Fossile brændstoffer og deres ekspansion
+- Fossile brændstoffer
 - Dårlig ledelsespraksis
 - Skadelige miljøpraksisser
-- Menneskerettighedsspørgsmål
+- Menneskerettigheder
 - ILO-brud
-- Overholdelse af internationale normer og konventioner
 - Landepolitik
 - Manglende klimaambitioner
 - Miljømæssige normbrud
@@ -1139,7 +1017,8 @@
 - Tjenester og forsyninger, der understøtter opretholdelse af bosættelser
 - Udnyttelse af naturressourcer, især vand og land
 - Termisk kul og dets udvinding
-- Usunde fødevarer</t>
+- Usunde fødevarer
+- Kul (kul-eksponering &gt; 5%</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
@@ -1158,14 +1037,12 @@
   <si>
     <t>- Arbejdstagerrettigheder og brud på internationale normer
 - Atomvåben og kontroversielle våben
-- Miljømæssige og biodiversitetsrelaterede problemstillinger
-- Menneskerettigheder og humanitære forhold
+- Miljø og biodiversitet
+- Menneskerettigheder
 - Negative effekter på klima og fossile brændstoffer
-- Ejendomsoverdragelse og involvering i problematiske sektorer som gambling og krydstogtskibe
-- Usunde fødevarer og skadelig ledelsespraksis
-- Overtrædelse af FN Global Compact principper
-- Overholdelse af internationale sanktioner og etik i forretningspraksis
-- Normbrud relateret til miljø og menneskerettigheder</t>
+- Ejendomsopkøb
+- Usunde fødevarer
+- Overtrædelse af FN Global Compact principper</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
@@ -1191,12 +1068,11 @@
 - Overtrædelse af FN Global Compact principper 3 og 4
 - Kontroversielle våben
 - Flyselskaber
-- Menneskerettighedskrænkelser
+- Menneskerettigheder
 - ILO-brud
 - Manglende klimaambitioner
-- Krænkelse af menneskerettigheder
 - Principal Adverse Impacts (PAI)
-- Involvering i tobaksprodukter
+- Tobak
 - Tilvejebringelse af serviceydelser til opretholdelse af bosættelser, herunder transport
 - Levering af sikkerhedstjenester til virksomheder i bosættelser
 - Anvendelse af naturressourcer som vand og land til erhvervsmæssige formål
@@ -1206,17 +1082,16 @@
   <si>
     <t>- Arbejdstagerrettigheder, herunder overtrædelser af ILO-konventioner.
 - Brud på grundlæggende rettigheder for arbejdstagere, i strid med FN Global Compact principper.
-- Involvering i kontroversielle våben.
-- Investment i flyselskaber.
-- Krænkelse af menneskerettigheder generelt.
+- Kontroversielle våben
+- Flyselskaber
+- Menneskerettigheder
 - Manglende indsats for klimaspørgsmål.
-- Normovertrædelser relateret til menneskerettigheder.
 - Negative konsekvenser for sociale forhold (Principal Adverse Impacts - PAI).
-- Involvering i tobaksprodukter som detailhandel.
+- Tobak
 - Levering af tjenesteydelser og forsyninger til bosættelser.
 - Forsyning af sikkerhedstjenester til virksomheder i bosættelser.
 - Utilstrækkelig forvaltning af naturressourcer (vand og land) i erhvervssammenhæng.
-- Tilbud af usunde fødevarer.</t>
+- Usunde fødevarer</t>
   </si>
   <si>
     <t>- Alkohol
@@ -1224,13 +1099,13 @@
 - Arbejdstagerrettigheder relateret til ILO-konventionen 87
 - Biodiversitet og dens påvirkninger
 - Brud på grundlæggende arbejdstagerrettigheder (FN Global Compact principper 3 og 4)
-- Kontroversielle våben, herunder hvid fosfor
+- Kontroversielle våben
 - Ejendomsopkøb
 - Flyselskaber
 - Fossile brændstoffer, herunder kul-udvidelse, fracking og overgangsproblematikker
 - Gambling
 - Skadelige miljøpraksisser
-- Menneskerettighedsproblematikker
+- Menneskerettigheder
 - ILO-brud
 - Integreret olie og gas
 - Internationale normer og konventioner
@@ -1244,7 +1119,7 @@
 - Normbrud relateret til miljø og menneskerettigheder
 - Olie og gas
 - Negative konsekvenser for mennesker og miljø 
-- Provision af tjenester og infrastruktur til opretholdelse af bosættelser
+- Støtte til tjenester og infrastruktur til opretholdelse af bosættelser
 - Termisk kul og dets udvinding
 - Usunde fødevarer
 - Våben</t>
@@ -1258,22 +1133,21 @@
 - Flyselskaber
 - Fossile brændstoffer og kuludvidelse
 - Gambling
-- God ledelsespraksis
-- Skadelige miljøpraksisser
-- Problemer med menneskerettigheder
+- Skadelige miljøpraksisser
+- Menneskerettigheder
 - ILO-brud
 - Normbrud i forhold til internationale konventioner
 - Involvering i kritisk produktion og aktiviteter
-- Konflikter relateret til Israel/Palæstina
+- Israel/Palæstina
 - Manglende klimaambitioner
 - Udnyttelse af naturressourcer, specielt vand og jord
 - Usunde fødevarer
-- Værktøjer til støtte for vedligeholdelse af bosættelser</t>
+- Støtte til tjenester og forsyninger i besættelsesområder, herunder transport</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
 - ILO-konventionen 87
-- EU sanktioner
+- EU-sanktioner
 - Fossil fuels
 - Kul med eksponering over 5%
 - Omsætning fra ukonventionel olie og gas, termisk kul eller arktisk boring over 5%
@@ -1282,7 +1156,7 @@
 - Israel/Palæstina
 - Sikkerhedsrisici
 - Ruslands invasion af Ukraine
-- Norms
+- Normer
 - SPU (Statens Pensionsfond)</t>
   </si>
   <si>
@@ -1296,7 +1170,6 @@
 - Flyselskab 
 - Fossile brændstoffer og fossil ekspansion 
 - Gambling 
-- God ledelsespraksis 
 - Skadelige miljøpraksisser 
 - Menneskerettighedsproblemer 
 - ILO-brud 
@@ -1335,7 +1208,6 @@
     <t>- Alkohol
 - Arbejdstagerrettigheder
 - Biodiversitet
-- Brud på grundlæggende menneskerettigheder
 - Kontroversielle våben
 - Dårlig regeringsførelse
 - EU-sanktioner
@@ -1357,7 +1229,7 @@
 - Olie og gasudvinding
 - Gambling
 - Principal Adverse Impacts (PAI)
-- Tobaksprodukter detailhandel
+- Tobak
 - Risikovurdering af ESG-forhold
 - Sikkerhedsforhold
 - Skat og EU's sortliste
@@ -1383,7 +1255,6 @@
 - Ikke-investeringsegnede lande
 - Fossile brændstoffer (kul, olie, gas)
 - Gambling
-- God ledelsespraksis
 - Skadelige miljøpraksisser
 - Menneskerettigheder
 - Internationale normer og konventioner
@@ -1399,107 +1270,100 @@
   <si>
     <t>- Brud på arbejdstagerrettigheder
 - Overtrædelser af ILO-konventioner
-- Menneskerettighedskrænkelser
-- Inddragelse i kontroversielle våben
+- Kontroversielle våben
 - Flyselskaber
 - Manglende overholdelse af FN Global Compact principper
-- Krænkelse af menneskerettigheder
-- Tidligere investeringer i tobaksprodukter
-- Betydelig negativ indvirkning på menneskerettigheder
-- Manglende klimaambitioner
-- Engagement i usunde fødevarer
+- Menneskerettigheder
+- Tobak
+- Manglende klimaambitioner
+- Usunde fødevarer
 - Inddragelse i termisk kuludvinding
-- Levering af tjenester til beskytning af beskedne bosættelser
+- Tjenester til brug i besatte områder
 - Levering af sikkerhedsudstyr og materialer til virksomheder i bosættelser</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
 - Brud på arbejdstagerrettigheder i overensstemmelse med FN Global Compact
-- Biodiversitet og tilknyttede miljøpåvirkninger
-- Kontroversielle våben
-- Ejendomsovertagelse
+- Biodiversitet
+- Kontroversielle våben
+- Ejendomsopkøb
 - Flyselskaber
 - Fossile brændstoffer
 - Gambling
 - Skadelige miljøpraksisser
-- Menneskerettigheder og relaterede spørgsmål
+- Menneskerettigheder
 - Overtrædelser af ILO-konventioner
 - Internationale normer og konventioner
 - Manglende klimaambitioner
 - Usunde fødevarer
-- Krænkelse af menneskerettigheder
 - Udstyr og tjenester til brug i besatte områder
 - Levering af sikkerhedstjenester og udstyr til virksomheder i besatte områder
 - Udvinding af termisk kul
-- Involvering i tobaksprodukter
+- Tobak
 - Krydstogtskibe
 - Våben</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder og brud herpå, herunder ILO-konventioner
-- Krænkelse af menneskerettigheder
 - Kontroversielle våben
 - Overholdelse af EU-sanktioner
-- Forhold til flyselskaber
-- Investeringer i fossile brændstoffer og transition til bæredygtige alternativer
+- Flyselskaber
+- Fossil brændstof og transition
 - Kul-eksponering over 5%
 - Manglende klimaambitioner
 - Omsætning fra ukonventionel olie og gas samt arktisk boring over 5%
-- Normovertrædelser relateret til menneskerettigheder
-- Samsyn med FN Global Compact principper
-- Forhold til Israel/Palæstina 
+- Menneskerettigheder
+- Israel/Palæstina 
 - Ruslands invasion af Ukraine
-- Usunde fødevarer og produkter relateret til tobak
+- Usunde fødevarer
 - Sikkerhedsrisici ved investeringer i besatte områder
-- Generel virksomhedsforvaltningsetik og internationale sanktioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Arbejdstagerrettigheder og relaterede brud 
+- Internationale sanktioner og forretningsetik</t>
+  </si>
+  <si>
+    <t>- Arbejdstagerrettigheder og relaterede brud 
 - Biodiversitet og skader på biodiversitet 
 - Brud på arbejdstagerrettigheder ifølge FN Global Compact 
 - Kontroversielle våben 
-- Investeringer i flyselskaber 
+- Flyselskaber 
 - Fossile brændstoffer og fossil ekspansion 
-- Spil og hasard 
+- Gambling 
 - Skadelige miljøpraksis 
-- Krænkelse af menneskerettigheder 
+- Menneskerettigheder 
 - Kul og eksponering for kul 
 - Manglende klimaambitioner 
-- Normovertrædelser vedrørende menneskerettigheder 
 - Negative primære konsekvenser (PAI) 
-- Investeringer i tobaksprodukter 
+- Tobak 
 - Tjenester, der støtter bosættelser 
 - Levering af sikkerhedstjenester til virksomheder i bosættelser 
 - Udnyttelse af naturressourcer, især vand og land 
-- Udtvungne fødevarer </t>
+- Usunde fødevarer 
+- Krydstogtskibe</t>
   </si>
   <si>
     <t>- Alkohol
 - Kontroversielle våben
 - Flyselskaber
-- Fossile brændstoffer (overordnet)
+- Fosstil brændstof
 - Transition fra fossile brændstoffer
 - Integreret olie og gas
 - Klimarelaterede forhold
-- Miljømæssige påvirkninger
-- Etiske normer (generelt)
-- Etiske normer relateret til fossile brændstoffer
+- Miljø
 - Olie
 - Principielle negative påvirkninger (PAI)
 - Tjenester og forsyninger relateret til opretholdelse af bosættelser, inklusiv transport</t>
   </si>
   <si>
     <t>- Flyselskaber
-- Israel/Palestina 
+- Israel/Palæstina 
 - Menneskerettigheder 
 - Principal Adverse Impacts (PAI)
 - Levering af tjenester og forsyninger, der støtter opretholdelsen af bosættelser, herunder transport 
-- Udtvinding af termisk kul 
+- Udvinding af termisk kul 
 - Usunde fødevarer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Biodiversitetspåvirkninger
+- Biodiversitet
 - Kontroversielle våben
 - Fossile brændstoffer
 - Udvidelse af fossile brændstoffer
@@ -1520,11 +1384,10 @@
 - Dårlig regeringsførelse og manglende overholdelse af internationale normer
 - EU-sanktioner og involvering i sanktionerede lande
 - Investeringer i fossil energi, herunder kul, olie og gas
-- Menneskerettighedskrænkelser og normbrud
+- Menneskerettigheder
 - Skat og skattemæssige problematikker
 - Low ESG performance og manglende klimaambitioner
-- Landeeksklusion baseret på investeringsegnede vurderinger
-- Kontroversielle aktiviteter som flyselskaber og krydstogtskibe
+- Flyselskaber
 - Normovertrædelser associeret med miljøforurening og sundhedsstandarder
 - Ingen relevant data.</t>
   </si>
@@ -1532,12 +1395,12 @@
     <t>- Arbejdstagerrettigheder og brud på internationale normer.
 - Miljømæssige konsekvenser og skader på biodiversitet.
 - Involvering i kontroversielle våben, herunder hvidt fosfor.
-- Ejendomsopkøb og deraf følgende juridiske og etiske problemstillinger.
+- Ejendomsopkøb
 - Investeringer i emerging markets, der ikke opfylder ESG-kriterier.
 - Aktiviteter relateret til fossil energi, herunder kuludvinding og fracking.
-- Problematikker vedrørende menneskerettigheder og human rights issues.
+- Menneskerettigheder
 - Negative konsekvenser for klimaet og manglende klimaambitioner.
-- Usunde fødevarer og gambling som eksklusionsårsager.</t>
+- Usunde fødevarer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
@@ -1547,16 +1410,15 @@
 - Ejendomsopkøb
 - Fossile brændstoffer (kul, olie, gas)
 - Miljømæssig praksis
-- Krænkelse af menneskerettigheder
+- Menneskerettigheder
 - Involvering i hvidt fosfor produktion
 - Manglende klimaambitioner
 - Usunde fødevarer
 - Utilfredsstillende ledelsespraksis
 - Konflikter med internationale normer og konventioner
-- Uretfærdig brug af naturressourcer
+- Anvendelse af naturressourcer (vand og land) til forretningsformål
 - Tjenester, der understøtter opretholdelse af bosættelser
-- Levering af sikkerhedstjenester til bosættelser
-- Indflydelse på sundhed og velvære gennem produkter og tjenester</t>
+- Levering af sikkerhedstjenester til bosættelser</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder, herunder brud på ILO-konventioner og FN Global Compact principper.
@@ -1568,15 +1430,14 @@
 - Deltagelse i fossile brændstoffer, herunder kul og fossil brændstofudvidelse.
 - Manglende overholdelse af internationale normer, især relateret til menneskerettigheder.
 - Problemer med god ledelsespraksis og normbrud.
-- Engagement i usunde fødevarer og relaterede produkter.
-- Ikke-overholdelse af principper om menneskerettigheder og klimapolitik.</t>
+- Usunde fødevarer</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
 - Brud på arbejdstagerrettigheder (f.eks. ILO-konventionen 87)
 - Biodiversitetsimplikationer
 - Kontroversielle våben
-- EU sanktioner
+- EU-sanktioner
 - Flyselskaber
 - Fossil energi (Transition og Fuel)
 - Skadelige miljøpraksisser
@@ -1584,13 +1445,13 @@
 - ILO-brud
 - Internationale sanktioner og forretningsetik
 - Israel/Palæstina
-- Krænkelse af menneskerettigheder
+- Menneskerettigheder
 - Kul (kul-eksponering &gt; 5%)
 - Manglende klimaambitioner
 - Normovertrædelser
 - Omsætning fra ukonventionel olie og gas, termisk kul eller arktisk boring &gt;5%
 - Principal Adverse Impacts (PAI)
-- Involvering i tobaksprodukter
+- Tobak
 - Ruslands invasion af Ukraine
 - Sikkerhedsforhold
 - Levering af tjenester og forsyninger til bosættelser
@@ -1601,7 +1462,7 @@
   </si>
   <si>
     <t>- Arbejdstagerrettigheder
-- Biodiversitet og dens konsekvenser
+- Biodiversitet
 - Brud på grundlæggende arbejdstagerrettigheder
 - Kontroversielle våben
 - EU-sanktioner
@@ -1611,13 +1472,13 @@
 - Fossile brændstoffer
 - Gambling
 - Skadelige miljøpraksisser
-- Menneskerettighedsproblemer
+- Menneskerettigheder
 - ILO-overtrædelser
 - Overtrædelse af internationale normer og konventioner
 - Konflikt med UN Global Compact princip nr. 10
 - Krydstogtskibe
 - Manglende klimaambitioner
-- Normbrud og normovertrædelser
+- Normer
 - Negative påvirkninger på principper 
 - Tjenester og forsyninger til opretholdelse af bosætninger
 - Udnyttelse af naturressourcer, især vand og land
@@ -1633,9 +1494,9 @@
 - Flyselskaber
 - Udvidelse af kulbaserede energikilder og fossil brændstofudvinding
 - Skadelig miljøpraksis
-- Problemer med menneskerettigheder
-- Investeringer relateret til Israel/Palæstina
-- Klimaændringer og tilknyttede risici
+- Menneskerettigheder
+- Israel/Palæstina
+- Klima
 - Investeringer i krydstogtskibe
 - Eksponering overfor kul og termisk kul (&gt;5%)
 - Omsætning fra ukonventionel olie og gas samt arktisk boring (&gt;5%)
@@ -1657,7 +1518,7 @@
 - Israel/Palæstina
 - Krydstogtskibe
 - Kul-eksponering over 5%
-- Uhensigtsmæssige fødevarer
+- Usunde fødevarer
 - Normer
 - Principal Adverse Impacts (PAI)
 - Termisk kuludvinding</t>
@@ -1667,16 +1528,16 @@
 - Brud på arbejdstagerrettigheder (inkl. ILO-konventionen 87)
 - Biodiversitet
 - Brud på FN Global Compact principperne 3 og 4
-- Kontroversielle våben (herunder hvid fosfor)
+- Kontroversielle våben
 - EU-sanktioner
 - Ejendomsopkøb
 - Emerging Markets statsobligationer, som ikke lever op til ESG-kriterier
 - Flyselskaber
 - Fossil energiproduktion (kuludvidelse og fossil brændstof)
 - Skadelig miljøpraksis
-- Menneskerettighedsspørgsmål
+- Menneskeretttigheder
 - Overtrædelser af internationale normer og konventioner
-- Klimagevinst og manglende klimaambitioner
+- Manglende klimaambitioner
 - Konflikt med UN Global Compact princip nr. 10
 - Landepolitik
 - Anvendelse af naturressourcer, især vand og land
@@ -1689,14 +1550,14 @@
     <t>- Arbejdstagerrettigheder
 - Brud på arbejdstagerrettigheder
 - Biodiversitet
-- Kontroversielle våben
+- Kontroversielle våben, herunder hvidt fosfor, herunder hvidt fosfor, herunder hvidt fosfor
 - EU-sanktioner
 - Ejendomsopkøb
 - Emerging Markets statsobligationer uden ESG-kriterier
 - Flyselskaber
 - Fossil brændstofudvidelse
 - Skadelige miljøpraksisser
-- Menneskerettighedsproblemer
+- Menneskerettigheder
 - Internationale normer og konventioner
 - Konflikter med UN Global Compact principper
 - Kul eksponering over 5%
@@ -1704,11 +1565,8 @@
 - Manglende klimaambitioner
 - Normbrud relateret til miljø
 - Usunde fødevarer
-  - Oplevelse af brud på menneskerettigheder
   - Negative miljøpåvirkninger
-  - Dårlige arbejdsforhold og praksisser
-  - Overtrædelser af internationale normer
-  - Engagement i kontroversielle aktiviteter og våbenproduktion</t>
+  - Dårlige arbejdsforhold og praksisser</t>
   </si>
   <si>
     <t>- Arbejdstagerrettigheder og relaterede brud (f.eks. ILO-konventionen 87)
@@ -1728,9 +1586,9 @@
 - Biodiversitet og negative konsekvenser for miljøet, herunder skadelige miljøpraksisser og manglende klimaambitioner.
 - Investeringer i kontroversielle våben og flyselskaber.
 - EU-sanktioner
-- Ejendomsopkøb og involvering i krænkende virksomhedsaktiviteter.
+- Ejendomsopkøb
 - Engagement i emerging markets statsobligationer, der ikke lever op til ESG-kriterier.
-- Deltagelse i gambling, usunde fødevarer og fossil fuel industri.
+- Gambling
 - Tilvejebringelse af sikkerhedsydelser til virksomheder i konfliktområder.
 - Anvendelse af naturressourcer, især vand og land, uden hensyntagen til bæredygtighed.
 - Involvering i tobaksprodukter og relaterede markeder.</t>
@@ -1741,7 +1599,7 @@
 - Atomvåben
 - Kontroversielle våben, herunder hvidt fosfor
 - Flyselskaber
-- Fossil energi og overgang til grøn energi
+- Fossil energi
 - Produktion af fossile brændstoffer
 - Gambling
 - Negativ påvirkning på klima og miljø
@@ -1757,30 +1615,25 @@
 - Biodiversitet og dens påvirkninger
 - Kontroversielle våben, herunder hvidt fosfor
 - Overholdelse af EU-sanktioner
-- Ejendomsopkøb i konfliktområder
+- Ejendomopkøb
 - Investeringer i emerging markets statsobligationer uden ESG-overholdelse
-- Flyselskaber med negative miljøpåvirkninger
+- Flyselskaber
 - Fossil energi og kul ekspansion
 - Gambling
-- God ledelsespraksis
 - Skadelig miljøpraksis
-- Menneskerettighedsproblemer
+- Menneskerettigheder
 - ILO-brud og brud på internationale normer
 - Konflikter med UN Global Compact principper
-- Krydstogtskibe og deres miljøeffekter
+- Krydstogtskibe
 - Kul-eksponering over 5%
-- Landepolitik uden bæredygtige tilgange
+- Landepolitik
 - Manglende klimaambitioner
 - Anvendelse af naturlige ressourcer på problematiske måder
 - Usunde fødevarer</t>
   </si>
   <si>
-    <t>- Eksklusionsårsager omfatter: 
-  - Kontroversielle våben
+    <t xml:space="preserve">  - Kontroversielle våben
   - Principale negative påvirkninger (PAI)
-- Overordnede årsager for eksklusion:
-  - Etik
-  - Sociale ansvar
   - Miljømæssig bæredygtighed</t>
   </si>
   <si>
@@ -1805,10 +1658,9 @@
     <t>- Overtrædelser af arbejdstagerrettigheder, herunder ILO-konventionen.
 - Brud på grundlæggende arbejdstagerrettigheder i strid med FN Global Compact principper.
 - Involvering i kontroversielle våben.
-- Investeringer i flyselskaber.
-- Krænkelse af menneskerettigheder og normer.
-- Manglende engagement i klimaindsats.
-- Negativ indvirkning på menneskerettigheder.
+- Flyselskaber
+- Menneskerettigheder.
+- Manglende klimaambitioner
 - Engagement i usunde fødevareprodukter.
 - Inddragelse i forsyning af sikkerhedstjenester til virksomheder i besatte områder.
 - Anvendelse af naturlige ressourcer, især vand og land, til erhvervsmæssige formål.</t>

</xml_diff>